<commit_message>
Script now checks if spreadsheet has already been logged. Please see updated excel file for an example
</commit_message>
<xml_diff>
--- a/obgyn.xlsx
+++ b/obgyn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1498E803-D246-4D90-AC48-3542F962F2A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0ADEDB8-34A0-4DA9-AFA4-09C679D3307F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7E74F0A7-02A5-44E8-A706-0746E0EECBF6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
   <si>
     <t>Abnormal labor</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>Other Gyn Procedure</t>
+  </si>
+  <si>
+    <t>DONE?</t>
   </si>
 </sst>
 </file>
@@ -306,7 +309,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -339,7 +342,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,21 +657,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1C5650-F933-470C-A08F-E0713328816C}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="topRight" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -678,8 +681,11 @@
       <c r="C1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -687,18 +693,24 @@
         <v>20</v>
       </c>
       <c r="C2" s="1">
-        <v>43885</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43899</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -706,20 +718,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>62</v>
       </c>
       <c r="C6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="D6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -727,142 +742,148 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>63</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>66</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -870,179 +891,178 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>83</v>
       </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>84</v>
       </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>86</v>
       </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>44</v>
       </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>45</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>47</v>
       </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>48</v>
       </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>54</v>
       </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>